<commit_message>
Atualização Map Conferencia LN - DEV, FAT e NFR
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_DEV.xlsx
+++ b/Documentação/Planilhas/Conferencia_DEV.xlsx
@@ -1227,13 +1227,38 @@
     <xf numFmtId="49" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1245,60 +1270,15 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1306,42 +1286,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1349,16 +1293,72 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1667,8 +1667,8 @@
   </sheetPr>
   <dimension ref="A2:AW36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="X10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -1724,20 +1724,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:49" ht="21">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="28"/>
+      <c r="B2" s="64"/>
       <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
       <c r="AR2" s="2"/>
     </row>
     <row r="3" spans="1:49" ht="21">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="28"/>
+      <c r="B3" s="64"/>
       <c r="C3" s="3" t="s">
         <v>276</v>
       </c>
@@ -1749,7 +1749,7 @@
     </row>
     <row r="5" spans="1:49" ht="21">
       <c r="A5" s="13"/>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="22" t="s">
         <v>277</v>
       </c>
       <c r="C5" s="3"/>
@@ -3410,602 +3410,602 @@
     </row>
     <row r="23" spans="1:49" ht="11.25" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="64" t="s">
+      <c r="C23" s="55"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="56"/>
+      <c r="H23" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="I23" s="64"/>
-      <c r="J23" s="64"/>
-      <c r="K23" s="64"/>
-      <c r="L23" s="64"/>
-      <c r="M23" s="64"/>
-      <c r="N23" s="64"/>
-      <c r="O23" s="64"/>
-      <c r="P23" s="64"/>
-      <c r="Q23" s="64"/>
-      <c r="R23" s="64"/>
-      <c r="S23" s="64"/>
-      <c r="T23" s="64"/>
-      <c r="U23" s="64"/>
-      <c r="V23" s="64"/>
-      <c r="W23" s="61" t="s">
+      <c r="I23" s="35"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="35"/>
+      <c r="L23" s="35"/>
+      <c r="M23" s="35"/>
+      <c r="N23" s="35"/>
+      <c r="O23" s="35"/>
+      <c r="P23" s="35"/>
+      <c r="Q23" s="35"/>
+      <c r="R23" s="35"/>
+      <c r="S23" s="35"/>
+      <c r="T23" s="35"/>
+      <c r="U23" s="35"/>
+      <c r="V23" s="35"/>
+      <c r="W23" s="43" t="s">
         <v>175</v>
       </c>
-      <c r="X23" s="61"/>
-      <c r="Y23" s="61"/>
-      <c r="Z23" s="61"/>
-      <c r="AA23" s="61"/>
-      <c r="AB23" s="61"/>
-      <c r="AC23" s="61"/>
-      <c r="AD23" s="61"/>
-      <c r="AE23" s="61"/>
-      <c r="AF23" s="61"/>
-      <c r="AG23" s="50" t="s">
+      <c r="X23" s="43"/>
+      <c r="Y23" s="43"/>
+      <c r="Z23" s="43"/>
+      <c r="AA23" s="43"/>
+      <c r="AB23" s="43"/>
+      <c r="AC23" s="43"/>
+      <c r="AD23" s="43"/>
+      <c r="AE23" s="43"/>
+      <c r="AF23" s="43"/>
+      <c r="AG23" s="23" t="s">
         <v>198</v>
       </c>
-      <c r="AH23" s="51"/>
-      <c r="AI23" s="52"/>
-      <c r="AJ23" s="26" t="s">
+      <c r="AH23" s="24"/>
+      <c r="AI23" s="25"/>
+      <c r="AJ23" s="65" t="s">
         <v>92</v>
       </c>
-      <c r="AK23" s="26" t="s">
+      <c r="AK23" s="65" t="s">
         <v>94</v>
       </c>
-      <c r="AL23" s="50" t="s">
+      <c r="AL23" s="23" t="s">
         <v>184</v>
       </c>
-      <c r="AM23" s="51"/>
-      <c r="AN23" s="51"/>
-      <c r="AO23" s="52"/>
-      <c r="AP23" s="29" t="s">
+      <c r="AM23" s="24"/>
+      <c r="AN23" s="24"/>
+      <c r="AO23" s="25"/>
+      <c r="AP23" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="AQ23" s="41"/>
-      <c r="AR23" s="41"/>
-      <c r="AS23" s="41"/>
-      <c r="AT23" s="30"/>
-      <c r="AU23" s="20" t="s">
+      <c r="AQ23" s="55"/>
+      <c r="AR23" s="55"/>
+      <c r="AS23" s="55"/>
+      <c r="AT23" s="56"/>
+      <c r="AU23" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="AV23" s="20" t="s">
+      <c r="AV23" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="AW23" s="49" t="s">
+      <c r="AW23" s="36" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:49" ht="11.25" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="64"/>
-      <c r="I24" s="64"/>
-      <c r="J24" s="64"/>
-      <c r="K24" s="64"/>
-      <c r="L24" s="64"/>
-      <c r="M24" s="64"/>
-      <c r="N24" s="64"/>
-      <c r="O24" s="64"/>
-      <c r="P24" s="64"/>
-      <c r="Q24" s="64"/>
-      <c r="R24" s="64"/>
-      <c r="S24" s="64"/>
-      <c r="T24" s="64"/>
-      <c r="U24" s="64"/>
-      <c r="V24" s="64"/>
-      <c r="W24" s="61"/>
-      <c r="X24" s="61"/>
-      <c r="Y24" s="61"/>
-      <c r="Z24" s="61"/>
-      <c r="AA24" s="61"/>
-      <c r="AB24" s="61"/>
-      <c r="AC24" s="61"/>
-      <c r="AD24" s="61"/>
-      <c r="AE24" s="61"/>
-      <c r="AF24" s="61"/>
-      <c r="AG24" s="53"/>
-      <c r="AH24" s="54"/>
-      <c r="AI24" s="55"/>
-      <c r="AJ24" s="26"/>
-      <c r="AK24" s="26"/>
-      <c r="AL24" s="53"/>
-      <c r="AM24" s="54"/>
-      <c r="AN24" s="54"/>
-      <c r="AO24" s="55"/>
-      <c r="AP24" s="31"/>
-      <c r="AQ24" s="42"/>
-      <c r="AR24" s="42"/>
-      <c r="AS24" s="42"/>
-      <c r="AT24" s="32"/>
-      <c r="AU24" s="21"/>
-      <c r="AV24" s="21"/>
-      <c r="AW24" s="49"/>
+      <c r="B24" s="57"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="59"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="35"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="35"/>
+      <c r="P24" s="35"/>
+      <c r="Q24" s="35"/>
+      <c r="R24" s="35"/>
+      <c r="S24" s="35"/>
+      <c r="T24" s="35"/>
+      <c r="U24" s="35"/>
+      <c r="V24" s="35"/>
+      <c r="W24" s="43"/>
+      <c r="X24" s="43"/>
+      <c r="Y24" s="43"/>
+      <c r="Z24" s="43"/>
+      <c r="AA24" s="43"/>
+      <c r="AB24" s="43"/>
+      <c r="AC24" s="43"/>
+      <c r="AD24" s="43"/>
+      <c r="AE24" s="43"/>
+      <c r="AF24" s="43"/>
+      <c r="AG24" s="26"/>
+      <c r="AH24" s="27"/>
+      <c r="AI24" s="28"/>
+      <c r="AJ24" s="65"/>
+      <c r="AK24" s="65"/>
+      <c r="AL24" s="26"/>
+      <c r="AM24" s="27"/>
+      <c r="AN24" s="27"/>
+      <c r="AO24" s="28"/>
+      <c r="AP24" s="57"/>
+      <c r="AQ24" s="58"/>
+      <c r="AR24" s="58"/>
+      <c r="AS24" s="58"/>
+      <c r="AT24" s="59"/>
+      <c r="AU24" s="52"/>
+      <c r="AV24" s="52"/>
+      <c r="AW24" s="36"/>
     </row>
     <row r="25" spans="1:49" ht="18" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="64"/>
-      <c r="I25" s="64"/>
-      <c r="J25" s="64"/>
-      <c r="K25" s="64"/>
-      <c r="L25" s="64"/>
-      <c r="M25" s="64"/>
-      <c r="N25" s="64"/>
-      <c r="O25" s="64"/>
-      <c r="P25" s="64"/>
-      <c r="Q25" s="64"/>
-      <c r="R25" s="64"/>
-      <c r="S25" s="64"/>
-      <c r="T25" s="64"/>
-      <c r="U25" s="64"/>
-      <c r="V25" s="64"/>
-      <c r="W25" s="61"/>
-      <c r="X25" s="61"/>
-      <c r="Y25" s="61"/>
-      <c r="Z25" s="61"/>
-      <c r="AA25" s="61"/>
-      <c r="AB25" s="61"/>
-      <c r="AC25" s="61"/>
-      <c r="AD25" s="61"/>
-      <c r="AE25" s="61"/>
-      <c r="AF25" s="61"/>
-      <c r="AG25" s="56"/>
-      <c r="AH25" s="57"/>
-      <c r="AI25" s="58"/>
-      <c r="AJ25" s="26"/>
-      <c r="AK25" s="26"/>
-      <c r="AL25" s="56"/>
-      <c r="AM25" s="57"/>
-      <c r="AN25" s="57"/>
-      <c r="AO25" s="58"/>
-      <c r="AP25" s="33"/>
-      <c r="AQ25" s="43"/>
-      <c r="AR25" s="43"/>
-      <c r="AS25" s="43"/>
-      <c r="AT25" s="34"/>
-      <c r="AU25" s="22"/>
-      <c r="AV25" s="22"/>
-      <c r="AW25" s="49"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="35"/>
+      <c r="J25" s="35"/>
+      <c r="K25" s="35"/>
+      <c r="L25" s="35"/>
+      <c r="M25" s="35"/>
+      <c r="N25" s="35"/>
+      <c r="O25" s="35"/>
+      <c r="P25" s="35"/>
+      <c r="Q25" s="35"/>
+      <c r="R25" s="35"/>
+      <c r="S25" s="35"/>
+      <c r="T25" s="35"/>
+      <c r="U25" s="35"/>
+      <c r="V25" s="35"/>
+      <c r="W25" s="43"/>
+      <c r="X25" s="43"/>
+      <c r="Y25" s="43"/>
+      <c r="Z25" s="43"/>
+      <c r="AA25" s="43"/>
+      <c r="AB25" s="43"/>
+      <c r="AC25" s="43"/>
+      <c r="AD25" s="43"/>
+      <c r="AE25" s="43"/>
+      <c r="AF25" s="43"/>
+      <c r="AG25" s="29"/>
+      <c r="AH25" s="30"/>
+      <c r="AI25" s="31"/>
+      <c r="AJ25" s="65"/>
+      <c r="AK25" s="65"/>
+      <c r="AL25" s="29"/>
+      <c r="AM25" s="30"/>
+      <c r="AN25" s="30"/>
+      <c r="AO25" s="31"/>
+      <c r="AP25" s="60"/>
+      <c r="AQ25" s="61"/>
+      <c r="AR25" s="61"/>
+      <c r="AS25" s="61"/>
+      <c r="AT25" s="62"/>
+      <c r="AU25" s="53"/>
+      <c r="AV25" s="53"/>
+      <c r="AW25" s="36"/>
     </row>
     <row r="26" spans="1:49" ht="11.25" customHeight="1">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="D26" s="23" t="s">
+      <c r="D26" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="E26" s="23" t="s">
+      <c r="E26" s="32" t="s">
         <v>165</v>
       </c>
-      <c r="F26" s="23" t="s">
+      <c r="F26" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="G26" s="23" t="s">
+      <c r="G26" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="H26" s="23" t="s">
+      <c r="H26" s="32" t="s">
         <v>191</v>
       </c>
-      <c r="I26" s="23" t="s">
+      <c r="I26" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="J26" s="23" t="s">
+      <c r="J26" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="K26" s="23" t="s">
+      <c r="K26" s="32" t="s">
         <v>194</v>
       </c>
-      <c r="L26" s="23" t="s">
+      <c r="L26" s="32" t="s">
         <v>197</v>
       </c>
-      <c r="M26" s="23" t="s">
+      <c r="M26" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="N26" s="23" t="s">
+      <c r="N26" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="O26" s="23" t="s">
+      <c r="O26" s="32" t="s">
         <v>250</v>
       </c>
-      <c r="P26" s="23" t="s">
+      <c r="P26" s="32" t="s">
         <v>275</v>
       </c>
-      <c r="Q26" s="23" t="s">
+      <c r="Q26" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="R26" s="27" t="s">
+      <c r="R26" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="S26" s="27" t="s">
+      <c r="S26" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="T26" s="27" t="s">
+      <c r="T26" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="U26" s="27" t="s">
+      <c r="U26" s="37" t="s">
         <v>169</v>
       </c>
-      <c r="V26" s="27" t="s">
+      <c r="V26" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="W26" s="44" t="s">
+      <c r="W26" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="X26" s="44" t="s">
+      <c r="X26" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="Y26" s="44" t="s">
+      <c r="Y26" s="38" t="s">
         <v>273</v>
       </c>
-      <c r="Z26" s="44" t="s">
+      <c r="Z26" s="38" t="s">
         <v>179</v>
       </c>
-      <c r="AA26" s="27" t="s">
+      <c r="AA26" s="37" t="s">
         <v>180</v>
       </c>
-      <c r="AB26" s="27" t="s">
+      <c r="AB26" s="37" t="s">
         <v>274</v>
       </c>
-      <c r="AC26" s="27" t="s">
+      <c r="AC26" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="AD26" s="27" t="s">
+      <c r="AD26" s="37" t="s">
         <v>182</v>
       </c>
-      <c r="AE26" s="23" t="s">
+      <c r="AE26" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="AF26" s="47" t="s">
+      <c r="AF26" s="63" t="s">
         <v>178</v>
       </c>
-      <c r="AG26" s="23" t="s">
+      <c r="AG26" s="32" t="s">
         <v>195</v>
       </c>
-      <c r="AH26" s="23" t="s">
+      <c r="AH26" s="32" t="s">
         <v>196</v>
       </c>
-      <c r="AI26" s="23" t="s">
+      <c r="AI26" s="32" t="s">
         <v>251</v>
       </c>
-      <c r="AJ26" s="35" t="s">
+      <c r="AJ26" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="AK26" s="38" t="s">
+      <c r="AK26" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="AL26" s="48" t="s">
+      <c r="AL26" s="44" t="s">
         <v>185</v>
       </c>
-      <c r="AM26" s="48" t="s">
+      <c r="AM26" s="44" t="s">
         <v>186</v>
       </c>
-      <c r="AN26" s="48" t="s">
+      <c r="AN26" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="AO26" s="48" t="s">
+      <c r="AO26" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="AP26" s="44" t="s">
+      <c r="AP26" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="AQ26" s="44" t="s">
+      <c r="AQ26" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="AR26" s="44" t="s">
+      <c r="AR26" s="38" t="s">
         <v>252</v>
       </c>
-      <c r="AS26" s="44" t="s">
+      <c r="AS26" s="38" t="s">
         <v>253</v>
       </c>
-      <c r="AT26" s="44" t="s">
+      <c r="AT26" s="38" t="s">
         <v>254</v>
       </c>
-      <c r="AU26" s="23" t="s">
+      <c r="AU26" s="32" t="s">
         <v>256</v>
       </c>
-      <c r="AV26" s="23" t="s">
+      <c r="AV26" s="32" t="s">
         <v>255</v>
       </c>
-      <c r="AW26" s="49"/>
+      <c r="AW26" s="36"/>
     </row>
     <row r="27" spans="1:49">
-      <c r="A27" s="24"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24"/>
-      <c r="Q27" s="24"/>
-      <c r="R27" s="27"/>
-      <c r="S27" s="27"/>
-      <c r="T27" s="27"/>
-      <c r="U27" s="27"/>
-      <c r="V27" s="27"/>
-      <c r="W27" s="45"/>
-      <c r="X27" s="45"/>
-      <c r="Y27" s="45"/>
-      <c r="Z27" s="45"/>
-      <c r="AA27" s="27"/>
-      <c r="AB27" s="27"/>
-      <c r="AC27" s="27"/>
-      <c r="AD27" s="27"/>
-      <c r="AE27" s="24"/>
-      <c r="AF27" s="47"/>
-      <c r="AG27" s="24"/>
-      <c r="AH27" s="24"/>
-      <c r="AI27" s="24"/>
-      <c r="AJ27" s="36"/>
-      <c r="AK27" s="39"/>
-      <c r="AL27" s="48"/>
-      <c r="AM27" s="48"/>
-      <c r="AN27" s="48"/>
-      <c r="AO27" s="48"/>
-      <c r="AP27" s="45"/>
-      <c r="AQ27" s="45"/>
-      <c r="AR27" s="59"/>
-      <c r="AS27" s="45"/>
-      <c r="AT27" s="45"/>
-      <c r="AU27" s="24"/>
-      <c r="AV27" s="24"/>
-      <c r="AW27" s="27" t="s">
+      <c r="A27" s="33"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="33"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="33"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="33"/>
+      <c r="O27" s="33"/>
+      <c r="P27" s="33"/>
+      <c r="Q27" s="33"/>
+      <c r="R27" s="37"/>
+      <c r="S27" s="37"/>
+      <c r="T27" s="37"/>
+      <c r="U27" s="37"/>
+      <c r="V27" s="37"/>
+      <c r="W27" s="39"/>
+      <c r="X27" s="39"/>
+      <c r="Y27" s="39"/>
+      <c r="Z27" s="39"/>
+      <c r="AA27" s="37"/>
+      <c r="AB27" s="37"/>
+      <c r="AC27" s="37"/>
+      <c r="AD27" s="37"/>
+      <c r="AE27" s="33"/>
+      <c r="AF27" s="63"/>
+      <c r="AG27" s="33"/>
+      <c r="AH27" s="33"/>
+      <c r="AI27" s="33"/>
+      <c r="AJ27" s="46"/>
+      <c r="AK27" s="49"/>
+      <c r="AL27" s="44"/>
+      <c r="AM27" s="44"/>
+      <c r="AN27" s="44"/>
+      <c r="AO27" s="44"/>
+      <c r="AP27" s="39"/>
+      <c r="AQ27" s="39"/>
+      <c r="AR27" s="41"/>
+      <c r="AS27" s="39"/>
+      <c r="AT27" s="39"/>
+      <c r="AU27" s="33"/>
+      <c r="AV27" s="33"/>
+      <c r="AW27" s="37" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="28" spans="1:49">
-      <c r="A28" s="24"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="24"/>
-      <c r="O28" s="24"/>
-      <c r="P28" s="24"/>
-      <c r="Q28" s="24"/>
-      <c r="R28" s="27"/>
-      <c r="S28" s="27"/>
-      <c r="T28" s="27"/>
-      <c r="U28" s="27"/>
-      <c r="V28" s="27"/>
-      <c r="W28" s="45"/>
-      <c r="X28" s="45"/>
-      <c r="Y28" s="45"/>
-      <c r="Z28" s="45"/>
-      <c r="AA28" s="27"/>
-      <c r="AB28" s="27"/>
-      <c r="AC28" s="27"/>
-      <c r="AD28" s="27"/>
-      <c r="AE28" s="24"/>
-      <c r="AF28" s="47"/>
-      <c r="AG28" s="24"/>
-      <c r="AH28" s="24"/>
-      <c r="AI28" s="24"/>
-      <c r="AJ28" s="36"/>
-      <c r="AK28" s="39"/>
-      <c r="AL28" s="48"/>
-      <c r="AM28" s="48"/>
-      <c r="AN28" s="48"/>
-      <c r="AO28" s="48"/>
-      <c r="AP28" s="45"/>
-      <c r="AQ28" s="45"/>
-      <c r="AR28" s="59"/>
-      <c r="AS28" s="45"/>
-      <c r="AT28" s="45"/>
-      <c r="AU28" s="24"/>
-      <c r="AV28" s="24"/>
-      <c r="AW28" s="27"/>
+      <c r="A28" s="33"/>
+      <c r="B28" s="33"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="33"/>
+      <c r="H28" s="33"/>
+      <c r="I28" s="33"/>
+      <c r="J28" s="33"/>
+      <c r="K28" s="33"/>
+      <c r="L28" s="33"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="33"/>
+      <c r="O28" s="33"/>
+      <c r="P28" s="33"/>
+      <c r="Q28" s="33"/>
+      <c r="R28" s="37"/>
+      <c r="S28" s="37"/>
+      <c r="T28" s="37"/>
+      <c r="U28" s="37"/>
+      <c r="V28" s="37"/>
+      <c r="W28" s="39"/>
+      <c r="X28" s="39"/>
+      <c r="Y28" s="39"/>
+      <c r="Z28" s="39"/>
+      <c r="AA28" s="37"/>
+      <c r="AB28" s="37"/>
+      <c r="AC28" s="37"/>
+      <c r="AD28" s="37"/>
+      <c r="AE28" s="33"/>
+      <c r="AF28" s="63"/>
+      <c r="AG28" s="33"/>
+      <c r="AH28" s="33"/>
+      <c r="AI28" s="33"/>
+      <c r="AJ28" s="46"/>
+      <c r="AK28" s="49"/>
+      <c r="AL28" s="44"/>
+      <c r="AM28" s="44"/>
+      <c r="AN28" s="44"/>
+      <c r="AO28" s="44"/>
+      <c r="AP28" s="39"/>
+      <c r="AQ28" s="39"/>
+      <c r="AR28" s="41"/>
+      <c r="AS28" s="39"/>
+      <c r="AT28" s="39"/>
+      <c r="AU28" s="33"/>
+      <c r="AV28" s="33"/>
+      <c r="AW28" s="37"/>
     </row>
     <row r="29" spans="1:49">
-      <c r="A29" s="24"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="24"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="24"/>
-      <c r="N29" s="24"/>
-      <c r="O29" s="24"/>
-      <c r="P29" s="24"/>
-      <c r="Q29" s="24"/>
-      <c r="R29" s="27"/>
-      <c r="S29" s="27"/>
-      <c r="T29" s="27"/>
-      <c r="U29" s="27"/>
-      <c r="V29" s="27"/>
-      <c r="W29" s="45"/>
-      <c r="X29" s="45"/>
-      <c r="Y29" s="45"/>
-      <c r="Z29" s="45"/>
-      <c r="AA29" s="27"/>
-      <c r="AB29" s="27"/>
-      <c r="AC29" s="27"/>
-      <c r="AD29" s="27"/>
-      <c r="AE29" s="24"/>
-      <c r="AF29" s="47"/>
-      <c r="AG29" s="24"/>
-      <c r="AH29" s="24"/>
-      <c r="AI29" s="24"/>
-      <c r="AJ29" s="36"/>
-      <c r="AK29" s="39"/>
-      <c r="AL29" s="48"/>
-      <c r="AM29" s="48"/>
-      <c r="AN29" s="48"/>
-      <c r="AO29" s="48"/>
-      <c r="AP29" s="45"/>
-      <c r="AQ29" s="45"/>
-      <c r="AR29" s="59"/>
-      <c r="AS29" s="45"/>
-      <c r="AT29" s="45"/>
-      <c r="AU29" s="24"/>
-      <c r="AV29" s="24"/>
-      <c r="AW29" s="27"/>
+      <c r="A29" s="33"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="33"/>
+      <c r="H29" s="33"/>
+      <c r="I29" s="33"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="33"/>
+      <c r="M29" s="33"/>
+      <c r="N29" s="33"/>
+      <c r="O29" s="33"/>
+      <c r="P29" s="33"/>
+      <c r="Q29" s="33"/>
+      <c r="R29" s="37"/>
+      <c r="S29" s="37"/>
+      <c r="T29" s="37"/>
+      <c r="U29" s="37"/>
+      <c r="V29" s="37"/>
+      <c r="W29" s="39"/>
+      <c r="X29" s="39"/>
+      <c r="Y29" s="39"/>
+      <c r="Z29" s="39"/>
+      <c r="AA29" s="37"/>
+      <c r="AB29" s="37"/>
+      <c r="AC29" s="37"/>
+      <c r="AD29" s="37"/>
+      <c r="AE29" s="33"/>
+      <c r="AF29" s="63"/>
+      <c r="AG29" s="33"/>
+      <c r="AH29" s="33"/>
+      <c r="AI29" s="33"/>
+      <c r="AJ29" s="46"/>
+      <c r="AK29" s="49"/>
+      <c r="AL29" s="44"/>
+      <c r="AM29" s="44"/>
+      <c r="AN29" s="44"/>
+      <c r="AO29" s="44"/>
+      <c r="AP29" s="39"/>
+      <c r="AQ29" s="39"/>
+      <c r="AR29" s="41"/>
+      <c r="AS29" s="39"/>
+      <c r="AT29" s="39"/>
+      <c r="AU29" s="33"/>
+      <c r="AV29" s="33"/>
+      <c r="AW29" s="37"/>
     </row>
     <row r="30" spans="1:49">
-      <c r="A30" s="24"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="24"/>
-      <c r="M30" s="24"/>
-      <c r="N30" s="24"/>
-      <c r="O30" s="24"/>
-      <c r="P30" s="24"/>
-      <c r="Q30" s="24"/>
-      <c r="R30" s="27"/>
-      <c r="S30" s="27"/>
-      <c r="T30" s="27"/>
-      <c r="U30" s="27"/>
-      <c r="V30" s="27"/>
-      <c r="W30" s="45"/>
-      <c r="X30" s="45"/>
-      <c r="Y30" s="45"/>
-      <c r="Z30" s="45"/>
-      <c r="AA30" s="27"/>
-      <c r="AB30" s="27"/>
-      <c r="AC30" s="27"/>
-      <c r="AD30" s="27"/>
-      <c r="AE30" s="24"/>
-      <c r="AF30" s="47"/>
-      <c r="AG30" s="24"/>
-      <c r="AH30" s="24"/>
-      <c r="AI30" s="24"/>
-      <c r="AJ30" s="36"/>
-      <c r="AK30" s="39"/>
-      <c r="AL30" s="48"/>
-      <c r="AM30" s="48"/>
-      <c r="AN30" s="48"/>
-      <c r="AO30" s="48"/>
-      <c r="AP30" s="45"/>
-      <c r="AQ30" s="45"/>
-      <c r="AR30" s="59"/>
-      <c r="AS30" s="45"/>
-      <c r="AT30" s="45"/>
-      <c r="AU30" s="24"/>
-      <c r="AV30" s="24"/>
-      <c r="AW30" s="27"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="33"/>
+      <c r="O30" s="33"/>
+      <c r="P30" s="33"/>
+      <c r="Q30" s="33"/>
+      <c r="R30" s="37"/>
+      <c r="S30" s="37"/>
+      <c r="T30" s="37"/>
+      <c r="U30" s="37"/>
+      <c r="V30" s="37"/>
+      <c r="W30" s="39"/>
+      <c r="X30" s="39"/>
+      <c r="Y30" s="39"/>
+      <c r="Z30" s="39"/>
+      <c r="AA30" s="37"/>
+      <c r="AB30" s="37"/>
+      <c r="AC30" s="37"/>
+      <c r="AD30" s="37"/>
+      <c r="AE30" s="33"/>
+      <c r="AF30" s="63"/>
+      <c r="AG30" s="33"/>
+      <c r="AH30" s="33"/>
+      <c r="AI30" s="33"/>
+      <c r="AJ30" s="46"/>
+      <c r="AK30" s="49"/>
+      <c r="AL30" s="44"/>
+      <c r="AM30" s="44"/>
+      <c r="AN30" s="44"/>
+      <c r="AO30" s="44"/>
+      <c r="AP30" s="39"/>
+      <c r="AQ30" s="39"/>
+      <c r="AR30" s="41"/>
+      <c r="AS30" s="39"/>
+      <c r="AT30" s="39"/>
+      <c r="AU30" s="33"/>
+      <c r="AV30" s="33"/>
+      <c r="AW30" s="37"/>
     </row>
     <row r="31" spans="1:49">
-      <c r="A31" s="25"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
-      <c r="M31" s="25"/>
-      <c r="N31" s="25"/>
-      <c r="O31" s="25"/>
-      <c r="P31" s="25"/>
-      <c r="Q31" s="25"/>
-      <c r="R31" s="27"/>
-      <c r="S31" s="27"/>
-      <c r="T31" s="27"/>
-      <c r="U31" s="27"/>
-      <c r="V31" s="27"/>
-      <c r="W31" s="46"/>
-      <c r="X31" s="46"/>
-      <c r="Y31" s="46"/>
-      <c r="Z31" s="46"/>
-      <c r="AA31" s="27"/>
-      <c r="AB31" s="27"/>
-      <c r="AC31" s="27"/>
-      <c r="AD31" s="27"/>
-      <c r="AE31" s="25"/>
-      <c r="AF31" s="47"/>
-      <c r="AG31" s="25"/>
-      <c r="AH31" s="25"/>
-      <c r="AI31" s="25"/>
-      <c r="AJ31" s="36"/>
-      <c r="AK31" s="39"/>
-      <c r="AL31" s="48"/>
-      <c r="AM31" s="48"/>
-      <c r="AN31" s="48"/>
-      <c r="AO31" s="48"/>
-      <c r="AP31" s="46"/>
-      <c r="AQ31" s="46"/>
-      <c r="AR31" s="60"/>
-      <c r="AS31" s="46"/>
-      <c r="AT31" s="46"/>
-      <c r="AU31" s="25"/>
-      <c r="AV31" s="25"/>
-      <c r="AW31" s="27"/>
+      <c r="A31" s="34"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+      <c r="I31" s="34"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="34"/>
+      <c r="L31" s="34"/>
+      <c r="M31" s="34"/>
+      <c r="N31" s="34"/>
+      <c r="O31" s="34"/>
+      <c r="P31" s="34"/>
+      <c r="Q31" s="34"/>
+      <c r="R31" s="37"/>
+      <c r="S31" s="37"/>
+      <c r="T31" s="37"/>
+      <c r="U31" s="37"/>
+      <c r="V31" s="37"/>
+      <c r="W31" s="40"/>
+      <c r="X31" s="40"/>
+      <c r="Y31" s="40"/>
+      <c r="Z31" s="40"/>
+      <c r="AA31" s="37"/>
+      <c r="AB31" s="37"/>
+      <c r="AC31" s="37"/>
+      <c r="AD31" s="37"/>
+      <c r="AE31" s="34"/>
+      <c r="AF31" s="63"/>
+      <c r="AG31" s="34"/>
+      <c r="AH31" s="34"/>
+      <c r="AI31" s="34"/>
+      <c r="AJ31" s="46"/>
+      <c r="AK31" s="49"/>
+      <c r="AL31" s="44"/>
+      <c r="AM31" s="44"/>
+      <c r="AN31" s="44"/>
+      <c r="AO31" s="44"/>
+      <c r="AP31" s="40"/>
+      <c r="AQ31" s="40"/>
+      <c r="AR31" s="42"/>
+      <c r="AS31" s="40"/>
+      <c r="AT31" s="40"/>
+      <c r="AU31" s="34"/>
+      <c r="AV31" s="34"/>
+      <c r="AW31" s="37"/>
     </row>
     <row r="32" spans="1:49">
-      <c r="AJ32" s="36"/>
-      <c r="AK32" s="39"/>
+      <c r="AJ32" s="46"/>
+      <c r="AK32" s="49"/>
     </row>
     <row r="33" spans="4:37">
       <c r="D33" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="AE33" s="62"/>
-      <c r="AJ33" s="36"/>
-      <c r="AK33" s="39"/>
+      <c r="AE33" s="20"/>
+      <c r="AJ33" s="46"/>
+      <c r="AK33" s="49"/>
     </row>
     <row r="34" spans="4:37" ht="258.75">
       <c r="D34" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="AE34" s="63"/>
-      <c r="AJ34" s="37"/>
-      <c r="AK34" s="40"/>
+      <c r="AE34" s="21"/>
+      <c r="AJ34" s="47"/>
+      <c r="AK34" s="50"/>
     </row>
     <row r="35" spans="4:37" ht="326.25">
       <c r="D35" s="9" t="s">
@@ -4019,6 +4019,52 @@
     </row>
   </sheetData>
   <mergeCells count="62">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="AJ23:AJ25"/>
+    <mergeCell ref="AK23:AK25"/>
+    <mergeCell ref="N26:N31"/>
+    <mergeCell ref="Z26:Z31"/>
+    <mergeCell ref="AA26:AA31"/>
+    <mergeCell ref="L26:L31"/>
+    <mergeCell ref="K26:K31"/>
+    <mergeCell ref="J26:J31"/>
+    <mergeCell ref="AC26:AC31"/>
+    <mergeCell ref="AD26:AD31"/>
+    <mergeCell ref="AE26:AE31"/>
+    <mergeCell ref="S26:S31"/>
+    <mergeCell ref="W26:W31"/>
+    <mergeCell ref="O26:O31"/>
+    <mergeCell ref="AU23:AU25"/>
+    <mergeCell ref="AV23:AV25"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="B26:B31"/>
+    <mergeCell ref="C26:C31"/>
+    <mergeCell ref="D26:D31"/>
+    <mergeCell ref="E26:E31"/>
+    <mergeCell ref="AP23:AT25"/>
+    <mergeCell ref="F26:F31"/>
+    <mergeCell ref="G26:G31"/>
+    <mergeCell ref="H26:H31"/>
+    <mergeCell ref="I26:I31"/>
+    <mergeCell ref="M26:M31"/>
+    <mergeCell ref="B23:G25"/>
+    <mergeCell ref="X26:X31"/>
+    <mergeCell ref="AF26:AF31"/>
+    <mergeCell ref="T26:T31"/>
+    <mergeCell ref="U26:U31"/>
+    <mergeCell ref="AS26:AS31"/>
+    <mergeCell ref="AI26:AI31"/>
+    <mergeCell ref="AO26:AO31"/>
+    <mergeCell ref="AP26:AP31"/>
+    <mergeCell ref="AQ26:AQ31"/>
+    <mergeCell ref="AG26:AG31"/>
+    <mergeCell ref="AH26:AH31"/>
+    <mergeCell ref="AL26:AL31"/>
+    <mergeCell ref="AM26:AM31"/>
+    <mergeCell ref="AN26:AN31"/>
+    <mergeCell ref="AJ26:AJ34"/>
+    <mergeCell ref="AK26:AK34"/>
     <mergeCell ref="AG23:AI25"/>
     <mergeCell ref="P26:P31"/>
     <mergeCell ref="H23:V25"/>
@@ -4035,52 +4081,6 @@
     <mergeCell ref="Y26:Y31"/>
     <mergeCell ref="AB26:AB31"/>
     <mergeCell ref="W23:AF25"/>
-    <mergeCell ref="T26:T31"/>
-    <mergeCell ref="U26:U31"/>
-    <mergeCell ref="AS26:AS31"/>
-    <mergeCell ref="AI26:AI31"/>
-    <mergeCell ref="AO26:AO31"/>
-    <mergeCell ref="AP26:AP31"/>
-    <mergeCell ref="AQ26:AQ31"/>
-    <mergeCell ref="AG26:AG31"/>
-    <mergeCell ref="AH26:AH31"/>
-    <mergeCell ref="AL26:AL31"/>
-    <mergeCell ref="AM26:AM31"/>
-    <mergeCell ref="AN26:AN31"/>
-    <mergeCell ref="AJ26:AJ34"/>
-    <mergeCell ref="AK26:AK34"/>
-    <mergeCell ref="AU23:AU25"/>
-    <mergeCell ref="AV23:AV25"/>
-    <mergeCell ref="A26:A31"/>
-    <mergeCell ref="B26:B31"/>
-    <mergeCell ref="C26:C31"/>
-    <mergeCell ref="D26:D31"/>
-    <mergeCell ref="E26:E31"/>
-    <mergeCell ref="AP23:AT25"/>
-    <mergeCell ref="F26:F31"/>
-    <mergeCell ref="G26:G31"/>
-    <mergeCell ref="H26:H31"/>
-    <mergeCell ref="I26:I31"/>
-    <mergeCell ref="M26:M31"/>
-    <mergeCell ref="B23:G25"/>
-    <mergeCell ref="X26:X31"/>
-    <mergeCell ref="AF26:AF31"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="AJ23:AJ25"/>
-    <mergeCell ref="AK23:AK25"/>
-    <mergeCell ref="N26:N31"/>
-    <mergeCell ref="Z26:Z31"/>
-    <mergeCell ref="AA26:AA31"/>
-    <mergeCell ref="L26:L31"/>
-    <mergeCell ref="K26:K31"/>
-    <mergeCell ref="J26:J31"/>
-    <mergeCell ref="AC26:AC31"/>
-    <mergeCell ref="AD26:AD31"/>
-    <mergeCell ref="AE26:AE31"/>
-    <mergeCell ref="S26:S31"/>
-    <mergeCell ref="W26:W31"/>
-    <mergeCell ref="O26:O31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>